<commit_message>
Design documents, aqi library, clue_pm25 versions
</commit_message>
<xml_diff>
--- a/docs/AQI workbook.xlsx
+++ b/docs/AQI workbook.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gloyer/Documents/pm25/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0240A93-7B7A-1240-94DD-067F65386C25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C372B72-BF1F-154E-B98C-BED8A4005CAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{CE7F1A1B-1DB8-024F-A4C1-4168E7AE1BC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -149,7 +149,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -208,16 +208,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -253,6 +253,45 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparison of PM2.5 AQI</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Purple</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Air, LRAPA, AQ&amp;U</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -293,11 +332,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$11</c:f>
+              <c:f>Sheet1!$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PM2.5 PA</c:v>
+                  <c:v>PA2.5 AQI</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -314,7 +353,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$12:$A$112</c:f>
               <c:numCache>
@@ -625,11 +664,323 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$B$112</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.833333333333336</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.666666666666671</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.382978723404257</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.021276595744681</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77.659574468085111</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88.297872340425528</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>98.936170212765958</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>111.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>123.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>136.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>148.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>152.36842105263159</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>157.63157894736841</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160.26315789473685</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>162.89473684210526</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>165.52631578947367</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>168.15789473684211</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>170.78947368421052</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>173.42105263157896</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>176.05263157894737</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>178.68421052631578</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>181.31578947368422</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>183.94736842105263</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>186.57894736842104</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>189.21052631578948</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>191.84210526315789</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>194.4736842105263</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>197.10526315789474</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>199.73684210526315</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>204.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>209.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>214.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>219.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>224.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>229.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>234.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>239.5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>244.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>249.5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>254.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>259.5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>264.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>269.5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>274.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>279.5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>284.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>289.5</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>294.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>299.5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>304.5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>309.5</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>314.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>319.5</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>324.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>329.5</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>334.5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>339.5</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>344.5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>349.5</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>354.5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>359.5</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>364.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>369.5</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>374.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>379.5</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>384.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>389.5</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>394.5</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>399.5</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>406.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>409.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>416.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>419.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>426.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>429.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>436.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>439.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>443</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>446.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>449.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>453</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>456.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>459.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>463</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>466.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>469.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>473</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>476.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>479.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>483</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>486.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>489.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>496.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>499.66666666666663</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4C2E-EF4D-AF29-47B26FCD9F79}"/>
+              <c16:uniqueId val="{00000000-1A3B-7247-8564-D7E0CA9C0627}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -638,11 +989,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$11</c:f>
+              <c:f>Sheet1!$D$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PA2.5 AQI</c:v>
+                  <c:v>LRAPA2.5  AQI</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -659,9 +1010,321 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$12:$A$112</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>425</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>435</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>465</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>485</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$B$112</c:f>
+              <c:f>Sheet1!$D$12:$D$112</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="101"/>
@@ -669,304 +1332,304 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.833333333333336</c:v>
+                  <c:v>7.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41.666666666666671</c:v>
+                  <c:v>18.083333333333336</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.382978723404257</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>67.021276595744681</c:v>
+                  <c:v>38.916666666666671</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>77.659574468085111</c:v>
+                  <c:v>49.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88.297872340425528</c:v>
+                  <c:v>54.978723404255319</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>98.936170212765958</c:v>
+                  <c:v>60.297872340425528</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>111.25</c:v>
+                  <c:v>65.61702127659575</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>123.75</c:v>
+                  <c:v>70.936170212765958</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>136.25</c:v>
+                  <c:v>76.255319148936167</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>148.75</c:v>
+                  <c:v>81.574468085106389</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>152.36842105263159</c:v>
+                  <c:v>86.893617021276597</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>155</c:v>
+                  <c:v>92.212765957446805</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>157.63157894736841</c:v>
+                  <c:v>97.531914893617028</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>160.26315789473685</c:v>
+                  <c:v>103.35000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>162.89473684210526</c:v>
+                  <c:v>109.60000000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>165.52631578947367</c:v>
+                  <c:v>115.85000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>168.15789473684211</c:v>
+                  <c:v>122.10000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>170.78947368421052</c:v>
+                  <c:v>128.35000000000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>173.42105263157896</c:v>
+                  <c:v>134.60000000000002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>176.05263157894737</c:v>
+                  <c:v>140.85000000000002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>178.68421052631578</c:v>
+                  <c:v>147.10000000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>181.31578947368422</c:v>
+                  <c:v>150.70526315789473</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>183.94736842105263</c:v>
+                  <c:v>152.02105263157895</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>186.57894736842104</c:v>
+                  <c:v>153.33684210526317</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>189.21052631578948</c:v>
+                  <c:v>154.65263157894736</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>191.84210526315789</c:v>
+                  <c:v>155.96842105263158</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>194.4736842105263</c:v>
+                  <c:v>157.2842105263158</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>197.10526315789474</c:v>
+                  <c:v>158.6</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>199.73684210526315</c:v>
+                  <c:v>159.91578947368421</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>204.5</c:v>
+                  <c:v>161.23157894736843</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>209.5</c:v>
+                  <c:v>162.54736842105262</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>214.5</c:v>
+                  <c:v>163.86315789473684</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>219.5</c:v>
+                  <c:v>165.17894736842106</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>224.5</c:v>
+                  <c:v>166.49473684210525</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>229.5</c:v>
+                  <c:v>167.81052631578947</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>234.5</c:v>
+                  <c:v>169.12631578947369</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>239.5</c:v>
+                  <c:v>170.44210526315788</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>244.5</c:v>
+                  <c:v>171.7578947368421</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>249.5</c:v>
+                  <c:v>173.07368421052632</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>254.5</c:v>
+                  <c:v>174.38947368421051</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>259.5</c:v>
+                  <c:v>175.70526315789473</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>264.5</c:v>
+                  <c:v>177.02105263157895</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>269.5</c:v>
+                  <c:v>178.33684210526314</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>274.5</c:v>
+                  <c:v>179.65263157894736</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>279.5</c:v>
+                  <c:v>180.96842105263158</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>284.5</c:v>
+                  <c:v>182.2842105263158</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>289.5</c:v>
+                  <c:v>183.6</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>294.5</c:v>
+                  <c:v>184.91578947368421</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>299.5</c:v>
+                  <c:v>186.2315789473684</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>304.5</c:v>
+                  <c:v>187.54736842105262</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>309.5</c:v>
+                  <c:v>188.86315789473684</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>314.5</c:v>
+                  <c:v>190.17894736842106</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>319.5</c:v>
+                  <c:v>191.49473684210525</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>324.5</c:v>
+                  <c:v>192.81052631578947</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>329.5</c:v>
+                  <c:v>194.12631578947369</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>334.5</c:v>
+                  <c:v>195.44210526315788</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>339.5</c:v>
+                  <c:v>196.7578947368421</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>344.5</c:v>
+                  <c:v>198.07368421052632</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>349.5</c:v>
+                  <c:v>199.38947368421054</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>354.5</c:v>
+                  <c:v>201.34</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>359.5</c:v>
+                  <c:v>203.84</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>364.5</c:v>
+                  <c:v>206.34</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>369.5</c:v>
+                  <c:v>208.84</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>374.5</c:v>
+                  <c:v>211.34</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>379.5</c:v>
+                  <c:v>213.84</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>384.5</c:v>
+                  <c:v>216.34</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>389.5</c:v>
+                  <c:v>218.84</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>394.5</c:v>
+                  <c:v>221.34</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>399.5</c:v>
+                  <c:v>223.84</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>403</c:v>
+                  <c:v>226.34</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>406.33333333333331</c:v>
+                  <c:v>228.84</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>409.66666666666669</c:v>
+                  <c:v>231.34</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>413</c:v>
+                  <c:v>233.84</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>416.33333333333331</c:v>
+                  <c:v>236.34</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>419.66666666666669</c:v>
+                  <c:v>238.84</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>423</c:v>
+                  <c:v>241.34</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>426.33333333333331</c:v>
+                  <c:v>243.84</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>429.66666666666669</c:v>
+                  <c:v>246.34</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>433</c:v>
+                  <c:v>248.84</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>436.33333333333331</c:v>
+                  <c:v>251.34</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>439.66666666666669</c:v>
+                  <c:v>253.84</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>443</c:v>
+                  <c:v>256.34000000000003</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>446.33333333333331</c:v>
+                  <c:v>258.84000000000003</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>449.66666666666669</c:v>
+                  <c:v>261.34000000000003</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>453</c:v>
+                  <c:v>263.84000000000003</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>456.33333333333331</c:v>
+                  <c:v>266.34000000000003</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>459.66666666666669</c:v>
+                  <c:v>268.84000000000003</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>463</c:v>
+                  <c:v>271.34000000000003</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>466.33333333333331</c:v>
+                  <c:v>273.84000000000003</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>469.66666666666663</c:v>
+                  <c:v>276.34000000000003</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>473</c:v>
+                  <c:v>278.84000000000003</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>476.33333333333331</c:v>
+                  <c:v>281.34000000000003</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>479.66666666666663</c:v>
+                  <c:v>283.84000000000003</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>483</c:v>
+                  <c:v>286.34000000000003</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>486.33333333333331</c:v>
+                  <c:v>288.84000000000003</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>489.66666666666663</c:v>
+                  <c:v>291.34000000000003</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>493</c:v>
+                  <c:v>293.84000000000003</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>496.33333333333331</c:v>
+                  <c:v>296.34000000000003</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>499.66666666666663</c:v>
+                  <c:v>298.84000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -974,7 +1637,664 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4C2E-EF4D-AF29-47B26FCD9F79}"/>
+              <c16:uniqueId val="{00000001-1A3B-7247-8564-D7E0CA9C0627}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AQ&amp;U2.5 AQI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$12:$A$112</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>425</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>435</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>465</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>485</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$12:$F$112</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>10.833333333333334</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.875000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.916666666666671</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54.574468085106382</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62.765957446808514</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70.957446808510639</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>79.148936170212778</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>87.340425531914889</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>95.531914893617028</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>104.375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>123.625</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>133.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>142.875</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150.52631578947367</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>152.55263157894737</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>154.57894736842104</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>156.60526315789474</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>158.63157894736841</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>160.65789473684211</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>162.68421052631578</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>164.71052631578948</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>166.73684210526315</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>168.76315789473682</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>170.78947368421052</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>172.81578947368422</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>174.84210526315789</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>176.86842105263156</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>178.89473684210526</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>180.92105263157896</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>182.94736842105263</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>184.9736842105263</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>189.0263157894737</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>191.05263157894737</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>193.07894736842104</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>195.10526315789474</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>197.13157894736844</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>199.15789473684211</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>202.25</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>206.1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>209.95</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>213.8</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>217.65</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>221.5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>225.35</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>229.2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>233.05</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>236.9</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>240.75</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>244.6</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>248.45</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>252.3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>256.14999999999998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>263.85000000000002</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>267.7</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>271.55</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>275.39999999999998</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>279.25</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>283.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>286.95</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>290.8</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>294.64999999999998</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>298.5</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>302.35000000000002</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>306.2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>310.05</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>313.90000000000003</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>317.75000000000006</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>321.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>325.45000000000005</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>329.3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>333.15000000000003</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>337.00000000000006</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>340.85</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>344.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>348.55</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>352.40000000000003</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>356.25000000000006</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>360.1</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>363.95000000000005</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>367.8</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>371.65000000000003</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>375.50000000000006</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>379.35</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>383.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>387.05</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>390.90000000000003</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>394.75000000000006</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>398.6</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>401.63333333333338</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>404.2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>406.76666666666671</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>409.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>411.90000000000003</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>414.4666666666667</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>417.03333333333336</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>419.6</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>422.16666666666669</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>424.73333333333335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1A3B-7247-8564-D7E0CA9C0627}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -987,16 +2307,72 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1554710032"/>
-        <c:axId val="1554711664"/>
+        <c:axId val="1823603856"/>
+        <c:axId val="1823857328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1554710032"/>
+        <c:axId val="1823603856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Raw Measurement (µg/m3)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1033,7 +2409,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1554711664"/>
+        <c:crossAx val="1823857328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1041,7 +2417,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1554711664"/>
+        <c:axId val="1823857328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1061,7 +2437,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>AQI</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1092,7 +2529,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1554710032"/>
+        <c:crossAx val="1823603856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1105,948 +2542,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$H$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>PM10.0 PA</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$12:$H$112</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="101"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>155</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>165</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>175</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>185</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>195</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>205</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>235</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>255</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>265</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>275</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>285</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>295</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>305</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>310</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>315</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>325</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>330</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>335</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>340</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>345</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>355</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>360</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>365</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>370</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>380</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>385</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>390</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>395</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>405</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>410</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>415</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>420</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>425</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>430</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>435</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>440</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>445</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>450</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>455</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>460</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>465</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>470</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>475</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>480</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>485</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>490</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>495</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2E44-F74C-8861-2ED15CEE9638}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$I$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>PA10.0 AQI</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$I$12:$I$112</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="101"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.545454545454545</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.0909090909090899</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.636363636363637</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18.18181818181818</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22.727272727272727</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>27.272727272727273</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>31.818181818181817</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>36.36363636363636</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>40.909090909090907</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>45.454545454545453</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>52.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>57.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>62.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>67.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>72.5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>77.5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>82.5</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>87.5</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>92.5</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>97.5</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>102.5</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>112.5</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>117.5</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>122.5</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>127.5</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>132.5</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>137.5</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>142.5</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>147.5</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>152.5</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>155</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>157.5</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>162.5</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>165</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>167.5</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>172.5</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>175</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>177.5</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>182.5</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>185</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>187.5</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>192.5</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>195</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>197.5</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>207.14285714285714</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>214.28571428571428</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>221.42857142857144</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>228.57142857142858</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>235.71428571428572</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>242.85714285714286</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>257.14285714285717</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>264.28571428571428</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>271.42857142857144</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>278.57142857142856</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>285.71428571428572</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>292.85714285714289</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>306.25</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>312.5</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>318.75</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>325</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>331.25</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>337.5</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>343.75</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>356.25</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>362.5</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>368.75</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>381.25</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>387.5</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>393.75</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2E44-F74C-8861-2ED15CEE9638}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1823494704"/>
-        <c:axId val="1823496336"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1823494704"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1823496336"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1823496336"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1823494704"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2121,46 +2617,6 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2716,543 +3172,27 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>124885</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>179919</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>336550</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>569384</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>78319</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{436F4B27-797F-0F4F-A96A-A029DFF2EFC4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4467E187-AAB8-7343-B4EB-B8A37647F3F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3265,42 +3205,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>349250</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7C6BE24-0F59-EF47-BDC0-C286EA5BCCF6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3608,8 +3512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0989D879-65DE-1740-8F77-B08A34D8641C}">
   <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F107" sqref="F107"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6114,7 +6018,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
-        <f t="shared" ref="A78:A135" si="14">A77+5</f>
+        <f t="shared" ref="A78:A112" si="14">A77+5</f>
         <v>330</v>
       </c>
       <c r="B78" s="5">

</xml_diff>